<commit_message>
feat(a-pagar): adiciona geração automática de parcelas para compras parceladas do caixa
</commit_message>
<xml_diff>
--- a/dados/Controle.xlsx
+++ b/dados/Controle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="17040" yWindow="0" windowWidth="29040" windowHeight="12480" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="1035" windowWidth="23250" windowHeight="12570" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Caixa" sheetId="1" state="visible" r:id="rId1"/>
@@ -168,10 +168,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -545,7 +545,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1104,19 +1104,57 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n"/>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="3" t="n"/>
-      <c r="F11" s="3" t="n"/>
-      <c r="G11" s="3" t="n"/>
-      <c r="H11" s="3" t="n"/>
-      <c r="I11" s="3" t="n"/>
-      <c r="J11" s="3" t="n"/>
-      <c r="K11" s="3" t="n"/>
-      <c r="L11" s="3" t="n"/>
-      <c r="M11" s="3" t="n"/>
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Compra</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>Parcelado</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="M11" s="6" t="n">
+        <v>46047.54166666666</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1129,7 +1167,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F306"/>
+  <dimension ref="A1:F407"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9080,6 +9118,2632 @@
         <v>31</v>
       </c>
       <c r="F306" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>100</v>
+      </c>
+      <c r="E307" t="n">
+        <v>31</v>
+      </c>
+      <c r="F307" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>1</v>
+      </c>
+      <c r="E308" t="n">
+        <v>30</v>
+      </c>
+      <c r="F308" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>1</v>
+      </c>
+      <c r="E309" t="n">
+        <v>31</v>
+      </c>
+      <c r="F309" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>1</v>
+      </c>
+      <c r="E310" t="n">
+        <v>31</v>
+      </c>
+      <c r="F310" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>100</v>
+      </c>
+      <c r="E311" t="n">
+        <v>31</v>
+      </c>
+      <c r="F311" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>1</v>
+      </c>
+      <c r="E312" t="n">
+        <v>30</v>
+      </c>
+      <c r="F312" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>1</v>
+      </c>
+      <c r="E313" t="n">
+        <v>31</v>
+      </c>
+      <c r="F313" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>1</v>
+      </c>
+      <c r="E314" t="n">
+        <v>31</v>
+      </c>
+      <c r="F314" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>1</v>
+      </c>
+      <c r="E315" t="n">
+        <v>31</v>
+      </c>
+      <c r="F315" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>100</v>
+      </c>
+      <c r="E316" t="n">
+        <v>31</v>
+      </c>
+      <c r="F316" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>100</v>
+      </c>
+      <c r="E317" t="n">
+        <v>31</v>
+      </c>
+      <c r="F317" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>100</v>
+      </c>
+      <c r="E318" t="n">
+        <v>31</v>
+      </c>
+      <c r="F318" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>1</v>
+      </c>
+      <c r="E319" t="n">
+        <v>30</v>
+      </c>
+      <c r="F319" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>1</v>
+      </c>
+      <c r="E320" t="n">
+        <v>31</v>
+      </c>
+      <c r="F320" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>1</v>
+      </c>
+      <c r="E321" t="n">
+        <v>31</v>
+      </c>
+      <c r="F321" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>1</v>
+      </c>
+      <c r="E322" t="n">
+        <v>31</v>
+      </c>
+      <c r="F322" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>100</v>
+      </c>
+      <c r="E323" t="n">
+        <v>31</v>
+      </c>
+      <c r="F323" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>1</v>
+      </c>
+      <c r="E324" t="n">
+        <v>30</v>
+      </c>
+      <c r="F324" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>1</v>
+      </c>
+      <c r="E325" t="n">
+        <v>31</v>
+      </c>
+      <c r="F325" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>1</v>
+      </c>
+      <c r="E326" t="n">
+        <v>31</v>
+      </c>
+      <c r="F326" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>1</v>
+      </c>
+      <c r="E327" t="n">
+        <v>31</v>
+      </c>
+      <c r="F327" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>100</v>
+      </c>
+      <c r="E328" t="n">
+        <v>31</v>
+      </c>
+      <c r="F328" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>1</v>
+      </c>
+      <c r="E329" t="n">
+        <v>30</v>
+      </c>
+      <c r="F329" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>1</v>
+      </c>
+      <c r="E330" t="n">
+        <v>31</v>
+      </c>
+      <c r="F330" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>1</v>
+      </c>
+      <c r="E331" t="n">
+        <v>31</v>
+      </c>
+      <c r="F331" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>1</v>
+      </c>
+      <c r="E332" t="n">
+        <v>31</v>
+      </c>
+      <c r="F332" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>100</v>
+      </c>
+      <c r="E333" t="n">
+        <v>31</v>
+      </c>
+      <c r="F333" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>1</v>
+      </c>
+      <c r="E334" t="n">
+        <v>30</v>
+      </c>
+      <c r="F334" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>1</v>
+      </c>
+      <c r="E335" t="n">
+        <v>31</v>
+      </c>
+      <c r="F335" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>1</v>
+      </c>
+      <c r="E336" t="n">
+        <v>31</v>
+      </c>
+      <c r="F336" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>1</v>
+      </c>
+      <c r="E337" t="n">
+        <v>31</v>
+      </c>
+      <c r="F337" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>100</v>
+      </c>
+      <c r="E338" t="n">
+        <v>31</v>
+      </c>
+      <c r="F338" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>1</v>
+      </c>
+      <c r="E339" t="n">
+        <v>30</v>
+      </c>
+      <c r="F339" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>1</v>
+      </c>
+      <c r="E340" t="n">
+        <v>31</v>
+      </c>
+      <c r="F340" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>1</v>
+      </c>
+      <c r="E341" t="n">
+        <v>31</v>
+      </c>
+      <c r="F341" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>1</v>
+      </c>
+      <c r="E342" t="n">
+        <v>31</v>
+      </c>
+      <c r="F342" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>100</v>
+      </c>
+      <c r="E343" t="n">
+        <v>31</v>
+      </c>
+      <c r="F343" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>1</v>
+      </c>
+      <c r="E344" t="n">
+        <v>30</v>
+      </c>
+      <c r="F344" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>1</v>
+      </c>
+      <c r="E345" t="n">
+        <v>31</v>
+      </c>
+      <c r="F345" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>1</v>
+      </c>
+      <c r="E346" t="n">
+        <v>31</v>
+      </c>
+      <c r="F346" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>1</v>
+      </c>
+      <c r="E347" t="n">
+        <v>31</v>
+      </c>
+      <c r="F347" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>100</v>
+      </c>
+      <c r="E348" t="n">
+        <v>31</v>
+      </c>
+      <c r="F348" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>1</v>
+      </c>
+      <c r="E349" t="n">
+        <v>30</v>
+      </c>
+      <c r="F349" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>1</v>
+      </c>
+      <c r="E350" t="n">
+        <v>31</v>
+      </c>
+      <c r="F350" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>1</v>
+      </c>
+      <c r="E351" t="n">
+        <v>31</v>
+      </c>
+      <c r="F351" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>1</v>
+      </c>
+      <c r="E352" t="n">
+        <v>31</v>
+      </c>
+      <c r="F352" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>100</v>
+      </c>
+      <c r="E353" t="n">
+        <v>31</v>
+      </c>
+      <c r="F353" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>1</v>
+      </c>
+      <c r="E354" t="n">
+        <v>30</v>
+      </c>
+      <c r="F354" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>1</v>
+      </c>
+      <c r="E355" t="n">
+        <v>31</v>
+      </c>
+      <c r="F355" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>1</v>
+      </c>
+      <c r="E356" t="n">
+        <v>31</v>
+      </c>
+      <c r="F356" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>1</v>
+      </c>
+      <c r="E357" t="n">
+        <v>31</v>
+      </c>
+      <c r="F357" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>100</v>
+      </c>
+      <c r="E358" t="n">
+        <v>31</v>
+      </c>
+      <c r="F358" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>1</v>
+      </c>
+      <c r="E359" t="n">
+        <v>30</v>
+      </c>
+      <c r="F359" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>1</v>
+      </c>
+      <c r="E360" t="n">
+        <v>31</v>
+      </c>
+      <c r="F360" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>1</v>
+      </c>
+      <c r="E361" t="n">
+        <v>31</v>
+      </c>
+      <c r="F361" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>1</v>
+      </c>
+      <c r="E362" t="n">
+        <v>31</v>
+      </c>
+      <c r="F362" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>100</v>
+      </c>
+      <c r="E363" t="n">
+        <v>31</v>
+      </c>
+      <c r="F363" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>1</v>
+      </c>
+      <c r="E364" t="n">
+        <v>30</v>
+      </c>
+      <c r="F364" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>1</v>
+      </c>
+      <c r="E365" t="n">
+        <v>31</v>
+      </c>
+      <c r="F365" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>1</v>
+      </c>
+      <c r="E366" t="n">
+        <v>31</v>
+      </c>
+      <c r="F366" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>1</v>
+      </c>
+      <c r="E367" t="n">
+        <v>31</v>
+      </c>
+      <c r="F367" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>100</v>
+      </c>
+      <c r="E368" t="n">
+        <v>31</v>
+      </c>
+      <c r="F368" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>1</v>
+      </c>
+      <c r="E369" t="n">
+        <v>30</v>
+      </c>
+      <c r="F369" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>1</v>
+      </c>
+      <c r="E370" t="n">
+        <v>31</v>
+      </c>
+      <c r="F370" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>1</v>
+      </c>
+      <c r="E371" t="n">
+        <v>31</v>
+      </c>
+      <c r="F371" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>1</v>
+      </c>
+      <c r="E372" t="n">
+        <v>31</v>
+      </c>
+      <c r="F372" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>100</v>
+      </c>
+      <c r="E373" t="n">
+        <v>31</v>
+      </c>
+      <c r="F373" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D374" t="n">
+        <v>1</v>
+      </c>
+      <c r="E374" t="n">
+        <v>30</v>
+      </c>
+      <c r="F374" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>1</v>
+      </c>
+      <c r="E375" t="n">
+        <v>31</v>
+      </c>
+      <c r="F375" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D376" t="n">
+        <v>1</v>
+      </c>
+      <c r="E376" t="n">
+        <v>31</v>
+      </c>
+      <c r="F376" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>1</v>
+      </c>
+      <c r="E377" t="n">
+        <v>31</v>
+      </c>
+      <c r="F377" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D378" t="n">
+        <v>100</v>
+      </c>
+      <c r="E378" t="n">
+        <v>31</v>
+      </c>
+      <c r="F378" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>1</v>
+      </c>
+      <c r="E379" t="n">
+        <v>30</v>
+      </c>
+      <c r="F379" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D380" t="n">
+        <v>1</v>
+      </c>
+      <c r="E380" t="n">
+        <v>31</v>
+      </c>
+      <c r="F380" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D381" t="n">
+        <v>1</v>
+      </c>
+      <c r="E381" t="n">
+        <v>31</v>
+      </c>
+      <c r="F381" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D382" t="n">
+        <v>1</v>
+      </c>
+      <c r="E382" t="n">
+        <v>31</v>
+      </c>
+      <c r="F382" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D383" t="n">
+        <v>100</v>
+      </c>
+      <c r="E383" t="n">
+        <v>31</v>
+      </c>
+      <c r="F383" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D384" t="n">
+        <v>1</v>
+      </c>
+      <c r="E384" t="n">
+        <v>30</v>
+      </c>
+      <c r="F384" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D385" t="n">
+        <v>1</v>
+      </c>
+      <c r="E385" t="n">
+        <v>31</v>
+      </c>
+      <c r="F385" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D386" t="n">
+        <v>1</v>
+      </c>
+      <c r="E386" t="n">
+        <v>31</v>
+      </c>
+      <c r="F386" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D387" t="n">
+        <v>1</v>
+      </c>
+      <c r="E387" t="n">
+        <v>31</v>
+      </c>
+      <c r="F387" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D388" t="n">
+        <v>100</v>
+      </c>
+      <c r="E388" t="n">
+        <v>31</v>
+      </c>
+      <c r="F388" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>1</v>
+      </c>
+      <c r="E389" t="n">
+        <v>30</v>
+      </c>
+      <c r="F389" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>1</v>
+      </c>
+      <c r="E390" t="n">
+        <v>31</v>
+      </c>
+      <c r="F390" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D391" t="n">
+        <v>1</v>
+      </c>
+      <c r="E391" t="n">
+        <v>31</v>
+      </c>
+      <c r="F391" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D392" t="n">
+        <v>1</v>
+      </c>
+      <c r="E392" t="n">
+        <v>31</v>
+      </c>
+      <c r="F392" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>100</v>
+      </c>
+      <c r="E393" t="n">
+        <v>31</v>
+      </c>
+      <c r="F393" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D394" t="n">
+        <v>1</v>
+      </c>
+      <c r="E394" t="n">
+        <v>30</v>
+      </c>
+      <c r="F394" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D395" t="n">
+        <v>1</v>
+      </c>
+      <c r="E395" t="n">
+        <v>31</v>
+      </c>
+      <c r="F395" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D396" t="n">
+        <v>1</v>
+      </c>
+      <c r="E396" t="n">
+        <v>31</v>
+      </c>
+      <c r="F396" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D397" t="n">
+        <v>1</v>
+      </c>
+      <c r="E397" t="n">
+        <v>31</v>
+      </c>
+      <c r="F397" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D398" t="n">
+        <v>100</v>
+      </c>
+      <c r="E398" t="n">
+        <v>31</v>
+      </c>
+      <c r="F398" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D399" t="n">
+        <v>1</v>
+      </c>
+      <c r="E399" t="n">
+        <v>30</v>
+      </c>
+      <c r="F399" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>1</v>
+      </c>
+      <c r="E400" t="n">
+        <v>31</v>
+      </c>
+      <c r="F400" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D401" t="n">
+        <v>1</v>
+      </c>
+      <c r="E401" t="n">
+        <v>31</v>
+      </c>
+      <c r="F401" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D402" t="n">
+        <v>1</v>
+      </c>
+      <c r="E402" t="n">
+        <v>31</v>
+      </c>
+      <c r="F402" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
+        <v>100</v>
+      </c>
+      <c r="E403" t="n">
+        <v>31</v>
+      </c>
+      <c r="F403" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D404" t="n">
+        <v>1</v>
+      </c>
+      <c r="E404" t="n">
+        <v>30</v>
+      </c>
+      <c r="F404" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D405" t="n">
+        <v>1</v>
+      </c>
+      <c r="E405" t="n">
+        <v>31</v>
+      </c>
+      <c r="F405" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D406" t="n">
+        <v>1</v>
+      </c>
+      <c r="E406" t="n">
+        <v>31</v>
+      </c>
+      <c r="F406" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D407" t="n">
+        <v>1</v>
+      </c>
+      <c r="E407" t="n">
+        <v>31</v>
+      </c>
+      <c r="F407" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -9746,7 +12410,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7935</v>
+        <v>10114</v>
       </c>
       <c r="E6" t="n">
         <v>31</v>
@@ -9766,7 +12430,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
@@ -9786,7 +12450,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
@@ -9806,7 +12470,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
@@ -9824,7 +12488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9860,7 +12524,12 @@
       </c>
       <c r="F1" s="9" t="inlineStr">
         <is>
-          <t>Data</t>
+          <t>Valor total pendente</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>Data vencimento</t>
         </is>
       </c>
     </row>
@@ -9884,7 +12553,10 @@
       <c r="E2" t="n">
         <v>50</v>
       </c>
-      <c r="F2" s="11" t="n">
+      <c r="F2" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G2" s="11" t="n">
         <v>46078.54166666666</v>
       </c>
     </row>
@@ -9908,7 +12580,10 @@
       <c r="E3" t="n">
         <v>50</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="F3" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G3" s="11" t="n">
         <v>46106.54166666666</v>
       </c>
     </row>
@@ -9932,7 +12607,10 @@
       <c r="E4" t="n">
         <v>50</v>
       </c>
-      <c r="F4" s="11" t="n">
+      <c r="F4" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G4" s="11" t="n">
         <v>46137.54166666666</v>
       </c>
     </row>
@@ -9956,7 +12634,10 @@
       <c r="E5" t="n">
         <v>50</v>
       </c>
-      <c r="F5" s="11" t="n">
+      <c r="F5" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G5" s="11" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>
@@ -9978,9 +12659,12 @@
         <v>12.5</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F6" s="11" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G6" s="11" t="n">
         <v>46078.54166666666</v>
       </c>
     </row>
@@ -10002,9 +12686,12 @@
         <v>12.5</v>
       </c>
       <c r="E7" t="n">
-        <v>50</v>
-      </c>
-      <c r="F7" s="11" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G7" s="11" t="n">
         <v>46106.54166666666</v>
       </c>
     </row>
@@ -10026,9 +12713,12 @@
         <v>12.5</v>
       </c>
       <c r="E8" t="n">
-        <v>50</v>
-      </c>
-      <c r="F8" s="11" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G8" s="11" t="n">
         <v>46137.54166666666</v>
       </c>
     </row>
@@ -10050,9 +12740,12 @@
         <v>12.5</v>
       </c>
       <c r="E9" t="n">
-        <v>50</v>
-      </c>
-      <c r="F9" s="11" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G9" s="11" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>
@@ -10070,9 +12763,16 @@
       <c r="C10" t="n">
         <v>1</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" s="11" t="n">
+      <c r="D10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="11" t="n">
         <v>46078.54166666666</v>
       </c>
     </row>
@@ -10090,9 +12790,16 @@
       <c r="C11" t="n">
         <v>2</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" s="11" t="n">
+      <c r="D11" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G11" s="11" t="n">
         <v>46106.54166666666</v>
       </c>
     </row>
@@ -10110,9 +12817,16 @@
       <c r="C12" t="n">
         <v>3</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" s="11" t="n">
+      <c r="D12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" t="n">
+        <v>25</v>
+      </c>
+      <c r="G12" s="11" t="n">
         <v>46137.54166666666</v>
       </c>
     </row>
@@ -10130,9 +12844,16 @@
       <c r="C13" t="n">
         <v>4</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" s="11" t="n">
+      <c r="D13" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>50</v>
+      </c>
+      <c r="F13" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G13" s="11" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>
@@ -10156,7 +12877,10 @@
       <c r="E14" t="n">
         <v>50</v>
       </c>
-      <c r="F14" s="11" t="n">
+      <c r="F14" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" s="11" t="n">
         <v>46078.54166666666</v>
       </c>
     </row>
@@ -10180,7 +12904,10 @@
       <c r="E15" t="n">
         <v>50</v>
       </c>
-      <c r="F15" s="11" t="n">
+      <c r="F15" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G15" s="11" t="n">
         <v>46106.54166666666</v>
       </c>
     </row>
@@ -10204,7 +12931,10 @@
       <c r="E16" t="n">
         <v>50</v>
       </c>
-      <c r="F16" s="11" t="n">
+      <c r="F16" t="n">
+        <v>25</v>
+      </c>
+      <c r="G16" s="11" t="n">
         <v>46137.54166666666</v>
       </c>
     </row>
@@ -10228,103 +12958,10 @@
       <c r="E17" t="n">
         <v>50</v>
       </c>
-      <c r="F17" s="11" t="n">
-        <v>46167.54166666666</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Maria</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" t="n">
+      <c r="F17" t="n">
         <v>12.5</v>
       </c>
-      <c r="E18" t="n">
-        <v>50</v>
-      </c>
-      <c r="F18" s="11" t="n">
-        <v>46078.54166666666</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Maria</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>2</v>
-      </c>
-      <c r="D19" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="E19" t="n">
-        <v>50</v>
-      </c>
-      <c r="F19" s="11" t="n">
-        <v>46106.54166666666</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Maria</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>3</v>
-      </c>
-      <c r="D20" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="E20" t="n">
-        <v>50</v>
-      </c>
-      <c r="F20" s="11" t="n">
-        <v>46137.54166666666</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Maria</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="E21" t="n">
-        <v>50</v>
-      </c>
-      <c r="F21" s="11" t="n">
+      <c r="G17" s="11" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>
@@ -10339,55 +12976,484 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L14:L15"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="9.140625" customWidth="1" style="3" min="1" max="1"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
-    <col width="17.7109375" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
-    <col width="12.5703125" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-    <col width="10.28515625" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
-    <col width="9.140625" customWidth="1" style="3" min="6" max="6"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>Cliente</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Parcelas Restantes</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>Parcela</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>Valor parcela</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>Valor total</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>Valor total pendente</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>Data vencimento</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F2" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G2" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E3" t="n">
+        <v>31</v>
+      </c>
+      <c r="F3" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G3" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E4" t="n">
+        <v>31</v>
+      </c>
+      <c r="F4" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E5" t="n">
+        <v>31</v>
+      </c>
+      <c r="F5" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G5" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E6" t="n">
+        <v>31</v>
+      </c>
+      <c r="F6" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E7" t="n">
+        <v>31</v>
+      </c>
+      <c r="F7" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F8" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E9" t="n">
+        <v>31</v>
+      </c>
+      <c r="F9" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F10" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E11" t="n">
+        <v>31</v>
+      </c>
+      <c r="F11" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F12" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E13" t="n">
+        <v>31</v>
+      </c>
+      <c r="F13" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E14" t="n">
+        <v>31</v>
+      </c>
+      <c r="F14" t="n">
+        <v>31</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E15" t="n">
+        <v>31</v>
+      </c>
+      <c r="F15" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G15" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E16" t="n">
+        <v>31</v>
+      </c>
+      <c r="F16" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G16" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E17" t="n">
+        <v>31</v>
+      </c>
+      <c r="F17" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G17" s="11" t="n">
+        <v>46167.54166666666</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: Criação da função de limpar caixa e correção de estrutura dos dataframe
</commit_message>
<xml_diff>
--- a/dados/Controle.xlsx
+++ b/dados/Controle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Caixa" sheetId="1" state="visible" r:id="rId1"/>
@@ -86,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -99,12 +99,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -510,67 +504,67 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Operação</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Participante</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Tamanho</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Sexo</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Desconto</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Forma Pag</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Parcelas</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>Valor unitario compra</t>
         </is>
       </c>
-      <c r="K1" s="7" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>Valor unitario venda</t>
         </is>
       </c>
-      <c r="L1" s="7" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>Valor recebido</t>
         </is>
       </c>
-      <c r="M1" s="7" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -605,7 +599,7 @@
       <c r="F2" t="n">
         <v>100</v>
       </c>
-      <c r="G2" s="12" t="n">
+      <c r="G2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -616,16 +610,16 @@
       <c r="I2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K2" s="12" t="n">
+      <c r="J2" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K2" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L2" s="12" t="n">
+      <c r="L2" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M2" s="13" t="n">
+      <c r="M2" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -658,7 +652,7 @@
       <c r="F3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="12" t="n">
+      <c r="G3" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -669,16 +663,16 @@
       <c r="I3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="12" t="n">
+      <c r="J3" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="K3" s="12" t="n">
+      <c r="K3" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L3" s="12" t="n">
+      <c r="L3" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M3" s="13" t="n">
+      <c r="M3" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -711,7 +705,7 @@
       <c r="F4" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="12" t="n">
+      <c r="G4" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -722,16 +716,16 @@
       <c r="I4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K4" s="12" t="n">
+      <c r="J4" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K4" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L4" s="12" t="n">
+      <c r="L4" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M4" s="13" t="n">
+      <c r="M4" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -762,7 +756,7 @@
       <c r="F5" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="12" t="n">
+      <c r="G5" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -773,16 +767,16 @@
       <c r="I5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K5" s="12" t="n">
+      <c r="J5" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K5" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L5" s="12" t="n">
+      <c r="L5" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M5" s="13" t="n">
+      <c r="M5" s="11" t="n">
         <v>46047.45833333334</v>
       </c>
     </row>
@@ -815,7 +809,7 @@
       <c r="F6" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="12" t="n">
+      <c r="G6" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -826,16 +820,16 @@
       <c r="I6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K6" s="12" t="n">
+      <c r="J6" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K6" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L6" s="12" t="n">
+      <c r="L6" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M6" s="13" t="n">
+      <c r="M6" s="11" t="n">
         <v>46047.5</v>
       </c>
     </row>
@@ -868,7 +862,7 @@
       <c r="F7" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="12" t="n">
+      <c r="G7" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="1" t="inlineStr">
@@ -879,16 +873,16 @@
       <c r="I7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J7" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K7" s="12" t="n">
+      <c r="J7" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K7" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L7" s="12" t="n">
+      <c r="L7" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M7" s="13" t="n">
+      <c r="M7" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -921,7 +915,7 @@
       <c r="F8" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="12" t="n">
+      <c r="G8" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="1" t="inlineStr">
@@ -932,16 +926,16 @@
       <c r="I8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K8" s="12" t="n">
+      <c r="J8" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K8" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L8" s="12" t="n">
+      <c r="L8" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M8" s="13" t="n">
+      <c r="M8" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -974,7 +968,7 @@
       <c r="F9" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="12" t="n">
+      <c r="G9" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="1" t="inlineStr">
@@ -985,16 +979,16 @@
       <c r="I9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="J9" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K9" s="12" t="n">
+      <c r="J9" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K9" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L9" s="12" t="n">
+      <c r="L9" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M9" s="13" t="n">
+      <c r="M9" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1027,7 +1021,7 @@
       <c r="F10" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="12" t="n">
+      <c r="G10" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="1" t="inlineStr">
@@ -1038,16 +1032,16 @@
       <c r="I10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="J10" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K10" s="12" t="n">
+      <c r="J10" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K10" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L10" s="12" t="n">
+      <c r="L10" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M10" s="13" t="n">
+      <c r="M10" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1080,7 +1074,7 @@
       <c r="F11" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="12" t="n">
+      <c r="G11" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="1" t="inlineStr">
@@ -1091,16 +1085,16 @@
       <c r="I11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="K11" s="12" t="n">
+      <c r="J11" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="K11" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L11" s="12" t="n">
+      <c r="L11" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="M11" s="13" t="n">
+      <c r="M11" s="11" t="n">
         <v>46047.58333333334</v>
       </c>
     </row>
@@ -1115,7 +1109,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1132,32 +1126,32 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Tamanho</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Sexo</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Valor unitario compra</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Data da compra</t>
         </is>
@@ -1182,10 +1176,10 @@
       <c r="D2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E2" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F2" s="13" t="n">
+      <c r="E2" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F2" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1208,10 +1202,10 @@
       <c r="D3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E3" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F3" s="13" t="n">
+      <c r="E3" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1234,10 +1228,10 @@
       <c r="D4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E4" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F4" s="13" t="n">
+      <c r="E4" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1260,10 +1254,10 @@
       <c r="D5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E5" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F5" s="13" t="n">
+      <c r="E5" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F5" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1286,10 +1280,10 @@
       <c r="D6" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E6" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F6" s="13" t="n">
+      <c r="E6" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F6" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1312,10 +1306,10 @@
       <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="12" t="n">
+      <c r="E7" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F7" s="13" t="n">
+      <c r="F7" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1338,10 +1332,10 @@
       <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F8" s="13" t="n">
+      <c r="E8" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F8" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1364,10 +1358,10 @@
       <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F9" s="13" t="n">
+      <c r="E9" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F9" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1390,10 +1384,10 @@
       <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F10" s="13" t="n">
+      <c r="E10" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F10" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1416,10 +1410,10 @@
       <c r="D11" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E11" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F11" s="13" t="n">
+      <c r="E11" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F11" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1442,10 +1436,10 @@
       <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="12" t="n">
+      <c r="E12" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F12" s="13" t="n">
+      <c r="F12" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1468,10 +1462,10 @@
       <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F13" s="13" t="n">
+      <c r="E13" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F13" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1494,10 +1488,10 @@
       <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F14" s="13" t="n">
+      <c r="E14" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F14" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1520,10 +1514,10 @@
       <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F15" s="13" t="n">
+      <c r="E15" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F15" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1546,10 +1540,10 @@
       <c r="D16" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E16" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F16" s="13" t="n">
+      <c r="E16" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F16" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1572,10 +1566,10 @@
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="12" t="n">
+      <c r="E17" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F17" s="13" t="n">
+      <c r="F17" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1598,10 +1592,10 @@
       <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F18" s="13" t="n">
+      <c r="E18" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F18" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1624,10 +1618,10 @@
       <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F19" s="13" t="n">
+      <c r="E19" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F19" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1650,10 +1644,10 @@
       <c r="D20" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E20" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F20" s="13" t="n">
+      <c r="E20" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F20" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1676,10 +1670,10 @@
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="12" t="n">
+      <c r="E21" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F21" s="13" t="n">
+      <c r="F21" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1702,10 +1696,10 @@
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F22" s="13" t="n">
+      <c r="E22" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F22" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1728,10 +1722,10 @@
       <c r="D23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F23" s="13" t="n">
+      <c r="E23" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F23" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1754,10 +1748,10 @@
       <c r="D24" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E24" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F24" s="13" t="n">
+      <c r="E24" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F24" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1780,10 +1774,10 @@
       <c r="D25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E25" s="12" t="n">
+      <c r="E25" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F25" s="13" t="n">
+      <c r="F25" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1806,10 +1800,10 @@
       <c r="D26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E26" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F26" s="13" t="n">
+      <c r="E26" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F26" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1832,10 +1826,10 @@
       <c r="D27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E27" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F27" s="13" t="n">
+      <c r="E27" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F27" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1858,10 +1852,10 @@
       <c r="D28" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F28" s="13" t="n">
+      <c r="E28" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F28" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1884,10 +1878,10 @@
       <c r="D29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E29" s="12" t="n">
+      <c r="E29" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F29" s="13" t="n">
+      <c r="F29" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1910,10 +1904,10 @@
       <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E30" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F30" s="13" t="n">
+      <c r="E30" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F30" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1936,10 +1930,10 @@
       <c r="D31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E31" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F31" s="13" t="n">
+      <c r="E31" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F31" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1962,10 +1956,10 @@
       <c r="D32" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E32" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F32" s="13" t="n">
+      <c r="E32" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F32" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1988,10 +1982,10 @@
       <c r="D33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="12" t="n">
+      <c r="E33" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F33" s="13" t="n">
+      <c r="F33" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2014,10 +2008,10 @@
       <c r="D34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E34" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F34" s="13" t="n">
+      <c r="E34" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F34" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2040,10 +2034,10 @@
       <c r="D35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E35" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F35" s="13" t="n">
+      <c r="E35" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F35" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2066,10 +2060,10 @@
       <c r="D36" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E36" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F36" s="13" t="n">
+      <c r="E36" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F36" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2092,10 +2086,10 @@
       <c r="D37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E37" s="12" t="n">
+      <c r="E37" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F37" s="13" t="n">
+      <c r="F37" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2118,10 +2112,10 @@
       <c r="D38" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E38" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F38" s="13" t="n">
+      <c r="E38" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F38" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2144,10 +2138,10 @@
       <c r="D39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E39" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F39" s="13" t="n">
+      <c r="E39" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F39" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2170,10 +2164,10 @@
       <c r="D40" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E40" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F40" s="13" t="n">
+      <c r="E40" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F40" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2196,10 +2190,10 @@
       <c r="D41" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E41" s="12" t="n">
+      <c r="E41" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F41" s="13" t="n">
+      <c r="F41" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2222,10 +2216,10 @@
       <c r="D42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E42" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F42" s="13" t="n">
+      <c r="E42" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F42" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2248,10 +2242,10 @@
       <c r="D43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E43" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F43" s="13" t="n">
+      <c r="E43" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F43" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2274,10 +2268,10 @@
       <c r="D44" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E44" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F44" s="13" t="n">
+      <c r="E44" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F44" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2300,10 +2294,10 @@
       <c r="D45" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E45" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F45" s="13" t="n">
+      <c r="E45" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F45" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2326,10 +2320,10 @@
       <c r="D46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E46" s="12" t="n">
+      <c r="E46" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F46" s="13" t="n">
+      <c r="F46" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2352,10 +2346,10 @@
       <c r="D47" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E47" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F47" s="13" t="n">
+      <c r="E47" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F47" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2378,10 +2372,10 @@
       <c r="D48" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E48" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F48" s="13" t="n">
+      <c r="E48" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F48" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2404,10 +2398,10 @@
       <c r="D49" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E49" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F49" s="13" t="n">
+      <c r="E49" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F49" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2430,10 +2424,10 @@
       <c r="D50" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E50" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F50" s="13" t="n">
+      <c r="E50" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F50" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2456,10 +2450,10 @@
       <c r="D51" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E51" s="12" t="n">
+      <c r="E51" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F51" s="13" t="n">
+      <c r="F51" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2482,10 +2476,10 @@
       <c r="D52" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F52" s="13" t="n">
+      <c r="E52" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F52" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2508,10 +2502,10 @@
       <c r="D53" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E53" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F53" s="13" t="n">
+      <c r="E53" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F53" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2534,10 +2528,10 @@
       <c r="D54" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E54" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F54" s="13" t="n">
+      <c r="E54" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F54" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2560,10 +2554,10 @@
       <c r="D55" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E55" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F55" s="13" t="n">
+      <c r="E55" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F55" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2586,10 +2580,10 @@
       <c r="D56" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E56" s="12" t="n">
+      <c r="E56" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F56" s="13" t="n">
+      <c r="F56" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2612,10 +2606,10 @@
       <c r="D57" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E57" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F57" s="13" t="n">
+      <c r="E57" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F57" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2638,10 +2632,10 @@
       <c r="D58" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E58" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F58" s="13" t="n">
+      <c r="E58" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F58" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2664,10 +2658,10 @@
       <c r="D59" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E59" s="12" t="n">
+      <c r="E59" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F59" s="13" t="n">
+      <c r="F59" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2690,10 +2684,10 @@
       <c r="D60" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E60" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F60" s="13" t="n">
+      <c r="E60" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F60" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2716,10 +2710,10 @@
       <c r="D61" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E61" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F61" s="13" t="n">
+      <c r="E61" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F61" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2742,10 +2736,10 @@
       <c r="D62" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E62" s="12" t="n">
+      <c r="E62" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F62" s="13" t="n">
+      <c r="F62" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2768,10 +2762,10 @@
       <c r="D63" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E63" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F63" s="13" t="n">
+      <c r="E63" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F63" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2794,10 +2788,10 @@
       <c r="D64" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E64" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F64" s="13" t="n">
+      <c r="E64" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F64" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2820,10 +2814,10 @@
       <c r="D65" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E65" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F65" s="13" t="n">
+      <c r="E65" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F65" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2846,10 +2840,10 @@
       <c r="D66" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E66" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F66" s="13" t="n">
+      <c r="E66" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F66" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2872,10 +2866,10 @@
       <c r="D67" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E67" s="12" t="n">
+      <c r="E67" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F67" s="13" t="n">
+      <c r="F67" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2898,10 +2892,10 @@
       <c r="D68" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E68" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F68" s="13" t="n">
+      <c r="E68" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F68" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2924,10 +2918,10 @@
       <c r="D69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E69" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F69" s="13" t="n">
+      <c r="E69" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F69" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2950,10 +2944,10 @@
       <c r="D70" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E70" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F70" s="13" t="n">
+      <c r="E70" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F70" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2976,10 +2970,10 @@
       <c r="D71" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E71" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F71" s="13" t="n">
+      <c r="E71" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F71" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3002,10 +2996,10 @@
       <c r="D72" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E72" s="12" t="n">
+      <c r="E72" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F72" s="13" t="n">
+      <c r="F72" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3028,10 +3022,10 @@
       <c r="D73" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E73" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F73" s="13" t="n">
+      <c r="E73" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F73" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3054,10 +3048,10 @@
       <c r="D74" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E74" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F74" s="13" t="n">
+      <c r="E74" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F74" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3080,10 +3074,10 @@
       <c r="D75" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E75" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F75" s="13" t="n">
+      <c r="E75" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F75" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3106,10 +3100,10 @@
       <c r="D76" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E76" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F76" s="13" t="n">
+      <c r="E76" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F76" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3132,10 +3126,10 @@
       <c r="D77" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E77" s="12" t="n">
+      <c r="E77" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F77" s="13" t="n">
+      <c r="F77" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3158,10 +3152,10 @@
       <c r="D78" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E78" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F78" s="13" t="n">
+      <c r="E78" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F78" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3184,10 +3178,10 @@
       <c r="D79" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E79" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F79" s="13" t="n">
+      <c r="E79" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F79" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3210,10 +3204,10 @@
       <c r="D80" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E80" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F80" s="13" t="n">
+      <c r="E80" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F80" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3236,10 +3230,10 @@
       <c r="D81" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E81" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F81" s="13" t="n">
+      <c r="E81" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F81" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3262,10 +3256,10 @@
       <c r="D82" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E82" s="12" t="n">
+      <c r="E82" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F82" s="13" t="n">
+      <c r="F82" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3288,10 +3282,10 @@
       <c r="D83" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E83" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F83" s="13" t="n">
+      <c r="E83" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F83" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3314,10 +3308,10 @@
       <c r="D84" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E84" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F84" s="13" t="n">
+      <c r="E84" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F84" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3340,10 +3334,10 @@
       <c r="D85" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E85" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F85" s="13" t="n">
+      <c r="E85" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F85" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3366,10 +3360,10 @@
       <c r="D86" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E86" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F86" s="13" t="n">
+      <c r="E86" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F86" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3392,10 +3386,10 @@
       <c r="D87" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E87" s="12" t="n">
+      <c r="E87" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F87" s="13" t="n">
+      <c r="F87" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3418,10 +3412,10 @@
       <c r="D88" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E88" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F88" s="13" t="n">
+      <c r="E88" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F88" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3444,10 +3438,10 @@
       <c r="D89" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E89" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F89" s="13" t="n">
+      <c r="E89" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F89" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3470,10 +3464,10 @@
       <c r="D90" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E90" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F90" s="13" t="n">
+      <c r="E90" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F90" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3496,10 +3490,10 @@
       <c r="D91" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E91" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F91" s="13" t="n">
+      <c r="E91" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F91" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3522,10 +3516,10 @@
       <c r="D92" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E92" s="12" t="n">
+      <c r="E92" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F92" s="13" t="n">
+      <c r="F92" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3548,10 +3542,10 @@
       <c r="D93" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E93" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F93" s="13" t="n">
+      <c r="E93" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F93" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3574,10 +3568,10 @@
       <c r="D94" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E94" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F94" s="13" t="n">
+      <c r="E94" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F94" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3600,10 +3594,10 @@
       <c r="D95" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E95" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F95" s="13" t="n">
+      <c r="E95" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F95" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3626,10 +3620,10 @@
       <c r="D96" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E96" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F96" s="13" t="n">
+      <c r="E96" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F96" s="11" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3652,10 +3646,10 @@
       <c r="D97" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E97" s="12" t="n">
+      <c r="E97" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="F97" s="13" t="n">
+      <c r="F97" s="11" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3678,10 +3672,10 @@
       <c r="D98" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E98" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F98" s="13" t="n">
+      <c r="E98" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F98" s="11" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3704,10 +3698,10 @@
       <c r="D99" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E99" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F99" s="13" t="n">
+      <c r="E99" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F99" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3730,10 +3724,660 @@
       <c r="D100" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E100" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F100" s="13" t="n">
+      <c r="E100" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F100" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B101" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C101" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E101" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F101" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B102" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C102" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F102" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B103" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C103" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D103" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F103" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B104" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C104" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F104" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B105" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C105" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D105" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F105" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B106" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C106" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D106" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E106" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F106" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B107" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C107" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D107" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E107" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F107" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B108" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C108" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D108" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F108" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B109" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C109" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D109" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E109" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F109" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B110" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C110" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D110" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E110" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F110" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B111" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C111" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D111" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E111" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F111" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B112" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C112" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D112" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F112" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B113" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C113" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D113" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F113" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B114" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C114" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D114" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F114" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B115" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C115" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D115" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E115" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F115" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B116" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C116" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D116" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E116" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F116" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B117" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C117" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D117" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E117" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F117" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B118" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C118" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D118" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F118" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B119" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C119" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D119" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E119" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F119" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B120" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C120" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E120" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F120" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B121" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C121" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D121" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E121" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F121" s="11" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B122" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C122" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E122" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F122" s="11" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B123" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C123" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D123" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E123" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F123" s="11" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B124" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C124" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D124" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F124" s="11" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B125" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C125" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D125" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E125" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F125" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3766,37 +4410,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Cliente</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Tamanho</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Sexo</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Valor unitario venda</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -3826,10 +4470,10 @@
       <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="12" t="n">
+      <c r="F2" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="11" t="n">
         <v>46047.5</v>
       </c>
     </row>
@@ -3857,10 +4501,10 @@
       <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="12" t="n">
+      <c r="F3" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="G3" s="13" t="n">
+      <c r="G3" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3888,10 +4532,10 @@
       <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="12" t="n">
+      <c r="F4" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="11" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3919,10 +4563,10 @@
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="12" t="n">
+      <c r="F5" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="11" t="n">
         <v>46047.58333333334</v>
       </c>
     </row>
@@ -3952,22 +4596,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Tamanho</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Valor unitario compra</t>
         </is>
@@ -3985,9 +4629,9 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>2682</v>
-      </c>
-      <c r="D2" s="12" t="n">
+        <v>3172</v>
+      </c>
+      <c r="D2" s="10" t="n">
         <v>31</v>
       </c>
     </row>
@@ -4003,9 +4647,9 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="D3" s="12" t="n">
+        <v>28</v>
+      </c>
+      <c r="D3" s="10" t="n">
         <v>30</v>
       </c>
     </row>
@@ -4021,9 +4665,9 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="D4" s="12" t="n">
+        <v>28</v>
+      </c>
+      <c r="D4" s="10" t="n">
         <v>31</v>
       </c>
     </row>
@@ -4038,7 +4682,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4056,37 +4700,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Cliente</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Parcela</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Valor parcela</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Valor total</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Valor total pendente</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Data vencimento</t>
         </is>
@@ -4106,16 +4750,16 @@
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="10" t="n">
         <v>12.5</v>
       </c>
-      <c r="E2" s="12" t="n">
+      <c r="E2" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="F2" s="12" t="n">
+      <c r="F2" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="11" t="n">
         <v>46078.54166666666</v>
       </c>
     </row>
@@ -4133,16 +4777,16 @@
       <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="10" t="n">
         <v>12.5</v>
       </c>
-      <c r="E3" s="12" t="n">
+      <c r="E3" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="F3" s="12" t="n">
+      <c r="F3" s="10" t="n">
         <v>37.5</v>
       </c>
-      <c r="G3" s="13" t="n">
+      <c r="G3" s="11" t="n">
         <v>46106.54166666666</v>
       </c>
     </row>
@@ -4160,16 +4804,16 @@
       <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="n">
+      <c r="D4" s="10" t="n">
         <v>12.5</v>
       </c>
-      <c r="E4" s="12" t="n">
+      <c r="E4" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="F4" s="12" t="n">
+      <c r="F4" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="11" t="n">
         <v>46137.54166666666</v>
       </c>
     </row>
@@ -4187,16 +4831,556 @@
       <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="12" t="n">
+      <c r="D5" s="10" t="n">
         <v>12.5</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="F5" s="12" t="n">
+      <c r="F5" s="10" t="n">
         <v>12.5</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F13" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F14" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F15" s="10" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G15" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="G16" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F17" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G17" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F18" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F19" s="10" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G19" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E20" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F20" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="G20" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F21" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G21" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E22" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F22" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G22" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E23" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F23" s="10" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G23" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E24" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F24" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="G24" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E25" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F25" s="10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G25" s="11" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>
@@ -4211,7 +5395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4228,37 +5412,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Participante</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Parcela</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Valor parcela</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Valor total</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Valor total pendente</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Data vencimento</t>
         </is>
@@ -4278,16 +5462,16 @@
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="10" t="n">
         <v>7.75</v>
       </c>
-      <c r="E2" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F2" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="G2" s="13" t="n">
+      <c r="E2" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F2" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2" s="11" t="n">
         <v>46078.54166666666</v>
       </c>
     </row>
@@ -4305,16 +5489,16 @@
       <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="10" t="n">
         <v>7.75</v>
       </c>
-      <c r="E3" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F3" s="12" t="n">
+      <c r="E3" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F3" s="10" t="n">
         <v>23.25</v>
       </c>
-      <c r="G3" s="13" t="n">
+      <c r="G3" s="11" t="n">
         <v>46106.54166666666</v>
       </c>
     </row>
@@ -4332,16 +5516,16 @@
       <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="n">
+      <c r="D4" s="10" t="n">
         <v>7.75</v>
       </c>
-      <c r="E4" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F4" s="12" t="n">
+      <c r="E4" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F4" s="10" t="n">
         <v>15.5</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="11" t="n">
         <v>46137.54166666666</v>
       </c>
     </row>
@@ -4359,16 +5543,556 @@
       <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="12" t="n">
+      <c r="D5" s="10" t="n">
         <v>7.75</v>
       </c>
-      <c r="E5" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="F5" s="12" t="n">
+      <c r="E5" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10" t="n">
         <v>7.75</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F10" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F13" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F14" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F15" s="10" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G15" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F16" s="10" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G16" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F17" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G17" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F18" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F19" s="10" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G19" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E20" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F20" s="10" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G20" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F21" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G21" s="11" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E22" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F22" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="G22" s="11" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E23" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F23" s="10" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G23" s="11" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E24" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F24" s="10" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G24" s="11" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E25" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F25" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G25" s="11" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>
@@ -4398,22 +6122,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Cpf</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Telefone</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Cidade</t>
         </is>

</xml_diff>

<commit_message>
Fix: correção para que atualize retorno dos dados para a função de formatação
</commit_message>
<xml_diff>
--- a/dados/Controle.xlsx
+++ b/dados/Controle.xlsx
@@ -1134,7 +1134,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1962,6 +1962,396 @@
         <v>46047.54166666666</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E32" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F32" s="13" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F33" s="13" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F34" s="13" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F35" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F36" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F37" s="13" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F38" s="13" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F39" s="13" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F40" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F41" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E42" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F42" s="13" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F43" s="13" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F44" s="13" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F45" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F46" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1973,7 +2363,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2396,6 +2786,378 @@
         <v>50</v>
       </c>
       <c r="G13" s="13" t="n">
+        <v>46047.58333333334</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" s="13" t="n">
+        <v>46047.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G15" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G17" s="13" t="n">
+        <v>46047.58333333334</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G18" s="13" t="n">
+        <v>46047.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G19" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G20" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G21" s="13" t="n">
+        <v>46047.58333333334</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G22" s="13" t="n">
+        <v>46047.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G23" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G24" s="13" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G25" s="13" t="n">
         <v>46047.58333333334</v>
       </c>
     </row>
@@ -2458,7 +3220,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>4442</v>
+        <v>5128</v>
       </c>
       <c r="D2" s="12" t="n">
         <v>31</v>
@@ -2476,7 +3238,7 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D3" s="12" t="n">
         <v>30</v>
@@ -2494,7 +3256,7 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D4" s="12" t="n">
         <v>31</v>
@@ -2511,7 +3273,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4617,6 +5379,330 @@
         <v>46167.54166666666</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E78" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F78" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G78" s="13" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D79" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E79" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F79" s="12" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G79" s="13" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D80" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E80" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F80" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="G80" s="13" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D81" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E81" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F81" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G81" s="13" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E82" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F82" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G82" s="13" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D83" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E83" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F83" s="12" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G83" s="13" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D84" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E84" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F84" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="G84" s="13" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D85" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E85" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F85" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G85" s="13" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E86" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F86" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="G86" s="13" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D87" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E87" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F87" s="12" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G87" s="13" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D88" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E88" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F88" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="G88" s="13" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D89" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E89" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F89" s="12" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G89" s="13" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4628,7 +5714,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6622,6 +7708,330 @@
         <v>7.75</v>
       </c>
       <c r="G73" s="13" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E74" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F74" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="G74" s="13" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D75" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E75" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F75" s="12" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G75" s="13" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D76" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E76" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F76" s="12" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G76" s="13" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D77" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E77" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F77" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G77" s="13" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E78" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F78" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="G78" s="13" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D79" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E79" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F79" s="12" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G79" s="13" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D80" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E80" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F80" s="12" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G80" s="13" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D81" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E81" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F81" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G81" s="13" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E82" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F82" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="G82" s="13" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D83" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E83" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F83" s="12" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G83" s="13" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D84" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E84" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F84" s="12" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G84" s="13" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D85" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E85" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="F85" s="12" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G85" s="13" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Separa Relatorio final de Compras e Vendas realizadas do lançamento diario
</commit_message>
<xml_diff>
--- a/dados/Controle.xlsx
+++ b/dados/Controle.xlsx
@@ -1159,7 +1159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4015,6 +4015,630 @@
         <v>46047.54166666666</v>
       </c>
     </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B110" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C110" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D110" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E110" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F110" s="9" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B111" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C111" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D111" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F111" s="9" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B112" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C112" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D112" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F112" s="9" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B113" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C113" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D113" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F113" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B114" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C114" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D114" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F114" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>Compra C</t>
+        </is>
+      </c>
+      <c r="B115" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C115" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D115" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E115" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F115" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B116" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C116" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D116" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E116" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F116" s="9" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B117" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C117" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D117" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E117" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F117" s="9" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B118" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C118" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D118" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F118" s="9" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B119" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C119" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D119" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E119" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F119" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B120" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C120" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E120" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F120" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>Compra C</t>
+        </is>
+      </c>
+      <c r="B121" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C121" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D121" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E121" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F121" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B122" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C122" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D122" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E122" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F122" s="9" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B123" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C123" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D123" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E123" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F123" s="9" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B124" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C124" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D124" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F124" s="9" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B125" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C125" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D125" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E125" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F125" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B126" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C126" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D126" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E126" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F126" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>Compra C</t>
+        </is>
+      </c>
+      <c r="B127" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C127" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D127" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E127" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F127" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B128" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C128" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D128" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E128" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F128" s="9" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B129" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C129" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D129" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E129" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F129" s="9" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B130" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C130" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D130" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E130" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F130" s="9" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B131" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C131" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D131" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E131" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F131" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B132" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C132" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D132" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E132" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F132" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>Compra C</t>
+        </is>
+      </c>
+      <c r="B133" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C133" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D133" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F133" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4026,7 +4650,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6628,6 +7252,618 @@
         <v>31</v>
       </c>
       <c r="G84" s="9" t="n">
+        <v>46047.58333333334</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t>Venda A</t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D85" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>46047.45833333334</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D86" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E86" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G86" s="9" t="n">
+        <v>46047.5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D87" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E87" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D88" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E88" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G88" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D89" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E89" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F89" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v>46047.58333333334</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>Venda A</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D90" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E90" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F90" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G90" s="9" t="n">
+        <v>46047.45833333334</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D91" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E91" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F91" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G91" s="9" t="n">
+        <v>46047.5</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D92" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F92" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G92" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D93" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E93" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F93" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G93" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B94" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C94" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D94" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E94" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F94" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G94" s="9" t="n">
+        <v>46047.58333333334</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B95" s="1" t="inlineStr">
+        <is>
+          <t>Venda A</t>
+        </is>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D95" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F95" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G95" s="9" t="n">
+        <v>46047.45833333334</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B96" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C96" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D96" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E96" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G96" s="9" t="n">
+        <v>46047.5</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B97" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C97" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D97" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E97" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F97" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G97" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C98" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D98" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E98" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G98" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C99" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D99" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E99" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G99" s="9" t="n">
+        <v>46047.58333333334</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B100" s="1" t="inlineStr">
+        <is>
+          <t>Venda A</t>
+        </is>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D100" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E100" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G100" s="9" t="n">
+        <v>46047.45833333334</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="B101" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C101" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D101" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E101" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G101" s="9" t="n">
+        <v>46047.5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B102" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C102" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D102" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G102" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B103" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C103" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D103" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E103" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G103" s="9" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B104" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C104" s="1" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="D104" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F104" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G104" s="9" t="n">
         <v>46047.58333333334</v>
       </c>
     </row>
@@ -6690,7 +7926,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>12166</v>
+        <v>12558</v>
       </c>
       <c r="D2" s="8" t="n">
         <v>31</v>
@@ -6708,7 +7944,7 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D3" s="8" t="n">
         <v>30</v>
@@ -6726,7 +7962,7 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>31</v>
@@ -6744,7 +7980,7 @@
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>31</v>
@@ -6760,7 +7996,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>31</v>
@@ -6777,7 +8013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8775,6 +10011,438 @@
         <v>46167.54166666666</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E74" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F74" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="G74" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D75" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E75" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F75" s="8" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G75" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D76" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E76" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F76" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="G76" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D77" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E77" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F77" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G77" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E78" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F78" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="G78" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D79" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E79" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F79" s="8" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G79" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D80" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E80" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F80" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="G80" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D81" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E81" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F81" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G81" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E82" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F82" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="G82" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D83" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E83" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F83" s="8" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D84" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E84" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F84" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="G84" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D85" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E85" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F85" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E86" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F86" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="G86" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D87" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E87" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F87" s="8" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D88" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E88" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F88" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="G88" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D89" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E89" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F89" s="8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -8786,7 +10454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10780,6 +12448,438 @@
         <v>7.75</v>
       </c>
       <c r="G73" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E74" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F74" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G74" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D75" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E75" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F75" s="8" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G75" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D76" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E76" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F76" s="8" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G76" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D77" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E77" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F77" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G77" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E78" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F78" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G78" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D79" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E79" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F79" s="8" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G79" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D80" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E80" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F80" s="8" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G80" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D81" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E81" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F81" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G81" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E82" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F82" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G82" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D83" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E83" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F83" s="8" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D84" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E84" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F84" s="8" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G84" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D85" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E85" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F85" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>46167.54166666666</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E86" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F86" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G86" s="9" t="n">
+        <v>46078.54166666666</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D87" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E87" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F87" s="8" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>46106.54166666666</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D88" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E88" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F88" s="8" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G88" s="9" t="n">
+        <v>46137.54166666666</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>marcos</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D89" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E89" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F89" s="8" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="G89" s="9" t="n">
         <v>46167.54166666666</v>
       </c>
     </row>

</xml_diff>